<commit_message>
alles Dokumente fertig gestellt bis auf die Material Liste die folg am Nachmittag
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung Luminescence LED's.xlsx
+++ b/doc/Zeitplanung Luminescence LED's.xlsx
@@ -5,19 +5,20 @@
   <workbookPr codeName="DieseArbeitsmappe" showPivotChartFilter="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darvi\Documents\Luminescence LED's\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darvi\Documents\Luminescence-LED\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BB3940-D46D-4FBA-B28E-CE6719986B53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53385A00-AF3A-47AD-9C8F-21CB6A3BFDE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
-    <sheet name="Ist Arbeitszeit - Übersicht" sheetId="7" r:id="rId2"/>
+    <sheet name="Tabelle1" sheetId="8" r:id="rId2"/>
+    <sheet name="Ist Arbeitszeit - Übersicht" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Ist Arbeitszeit - Übersicht'!$A$1:$O$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Ist Arbeitszeit - Übersicht'!$A$1:$O$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Zeitplanung!$A$1:$T$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
   <si>
     <t>Nr.</t>
   </si>
@@ -255,6 +256,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Optimal</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Worst Case</t>
   </si>
 </sst>
 </file>
@@ -1534,13 +1544,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1549,7 +1559,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1608,13 +1618,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2121,8 +2131,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="136" zoomScaleNormal="136" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2719,11 +2729,11 @@
       </c>
       <c r="C9" s="41">
         <f>SUM(C10:C13)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -2824,9 +2834,9 @@
       <c r="AA10" s="58"/>
       <c r="AB10" s="53"/>
       <c r="AC10" s="54"/>
-      <c r="AD10" s="55"/>
-      <c r="AE10" s="55"/>
-      <c r="AF10" s="56"/>
+      <c r="AD10" s="54"/>
+      <c r="AE10" s="54"/>
+      <c r="AF10" s="54"/>
       <c r="AG10" s="57"/>
       <c r="AH10" s="58"/>
       <c r="AI10" s="53"/>
@@ -2865,10 +2875,12 @@
       <c r="B11" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="49"/>
+      <c r="C11" s="49">
+        <v>3</v>
+      </c>
       <c r="D11" s="83">
         <f>SUM(G11:BJ11)</f>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E11" s="50">
         <v>1</v>
@@ -2878,18 +2890,18 @@
       <c r="H11" s="60"/>
       <c r="I11" s="61"/>
       <c r="J11" s="61">
-        <v>8</v>
-      </c>
-      <c r="K11" s="85">
-        <v>8</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="85"/>
       <c r="L11" s="62"/>
       <c r="M11" s="58" t="s">
         <v>5</v>
       </c>
       <c r="N11" s="59"/>
       <c r="O11" s="60"/>
-      <c r="P11" s="61"/>
+      <c r="P11" s="61">
+        <v>0.5</v>
+      </c>
       <c r="Q11" s="61"/>
       <c r="R11" s="56"/>
       <c r="S11" s="57"/>
@@ -2905,9 +2917,9 @@
       <c r="AA11" s="58"/>
       <c r="AB11" s="59"/>
       <c r="AC11" s="60"/>
-      <c r="AD11" s="61"/>
-      <c r="AE11" s="61"/>
-      <c r="AF11" s="56"/>
+      <c r="AD11" s="60"/>
+      <c r="AE11" s="60"/>
+      <c r="AF11" s="60"/>
       <c r="AG11" s="57"/>
       <c r="AH11" s="58"/>
       <c r="AI11" s="59"/>
@@ -2961,7 +2973,9 @@
       <c r="H12" s="60"/>
       <c r="I12" s="61"/>
       <c r="J12" s="61"/>
-      <c r="K12" s="63"/>
+      <c r="K12" s="63">
+        <v>0</v>
+      </c>
       <c r="L12" s="57"/>
       <c r="M12" s="58"/>
       <c r="N12" s="59"/>
@@ -2980,9 +2994,9 @@
       <c r="AA12" s="58"/>
       <c r="AB12" s="59"/>
       <c r="AC12" s="60"/>
-      <c r="AD12" s="61"/>
-      <c r="AE12" s="61"/>
-      <c r="AF12" s="63"/>
+      <c r="AD12" s="60"/>
+      <c r="AE12" s="60"/>
+      <c r="AF12" s="60"/>
       <c r="AG12" s="57"/>
       <c r="AH12" s="58"/>
       <c r="AI12" s="59"/>
@@ -3054,11 +3068,11 @@
       <c r="AA13" s="67"/>
       <c r="AB13" s="59"/>
       <c r="AC13" s="60"/>
-      <c r="AD13" s="55"/>
-      <c r="AE13" s="55"/>
-      <c r="AF13" s="55"/>
-      <c r="AG13" s="66"/>
-      <c r="AH13" s="67"/>
+      <c r="AD13" s="60"/>
+      <c r="AE13" s="60"/>
+      <c r="AF13" s="60"/>
+      <c r="AG13" s="57"/>
+      <c r="AH13" s="58"/>
       <c r="AI13" s="59"/>
       <c r="AJ13" s="60"/>
       <c r="AK13" s="55"/>
@@ -3097,11 +3111,11 @@
       </c>
       <c r="C14" s="41">
         <f>SUM(C15:C17)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D14" s="42">
         <f>SUM(D15:D17)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="31"/>
@@ -3169,10 +3183,12 @@
       <c r="B15" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="49"/>
+      <c r="C15" s="49">
+        <v>5</v>
+      </c>
       <c r="D15" s="83">
         <f>SUM(G15:BJ15)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="89" t="s">
@@ -3182,16 +3198,18 @@
       <c r="H15" s="54"/>
       <c r="I15" s="68"/>
       <c r="J15" s="87">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K15" s="63">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L15" s="57"/>
       <c r="M15" s="58"/>
       <c r="N15" s="53"/>
       <c r="O15" s="54"/>
-      <c r="P15" s="55"/>
+      <c r="P15" s="55">
+        <v>3</v>
+      </c>
       <c r="Q15" s="55"/>
       <c r="R15" s="56"/>
       <c r="S15" s="57"/>
@@ -3205,9 +3223,9 @@
       <c r="AA15" s="58"/>
       <c r="AB15" s="53"/>
       <c r="AC15" s="54"/>
-      <c r="AD15" s="55"/>
-      <c r="AE15" s="55"/>
-      <c r="AF15" s="56"/>
+      <c r="AD15" s="54"/>
+      <c r="AE15" s="54"/>
+      <c r="AF15" s="54"/>
       <c r="AG15" s="57"/>
       <c r="AH15" s="58"/>
       <c r="AI15" s="53"/>
@@ -3276,9 +3294,9 @@
       <c r="AA16" s="58"/>
       <c r="AB16" s="59"/>
       <c r="AC16" s="60"/>
-      <c r="AD16" s="55"/>
-      <c r="AE16" s="55"/>
-      <c r="AF16" s="56"/>
+      <c r="AD16" s="60"/>
+      <c r="AE16" s="60"/>
+      <c r="AF16" s="60"/>
       <c r="AG16" s="57"/>
       <c r="AH16" s="58"/>
       <c r="AI16" s="59"/>
@@ -3343,11 +3361,11 @@
       <c r="Y17" s="56"/>
       <c r="Z17" s="57"/>
       <c r="AA17" s="58"/>
-      <c r="AB17" s="69"/>
-      <c r="AC17" s="70"/>
-      <c r="AD17" s="55"/>
-      <c r="AE17" s="55"/>
-      <c r="AF17" s="56"/>
+      <c r="AB17" s="59"/>
+      <c r="AC17" s="60"/>
+      <c r="AD17" s="60"/>
+      <c r="AE17" s="60"/>
+      <c r="AF17" s="60"/>
       <c r="AG17" s="57"/>
       <c r="AH17" s="58"/>
       <c r="AI17" s="69"/>
@@ -3388,11 +3406,11 @@
       </c>
       <c r="C18" s="41">
         <f>SUM(C19:C30)</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3460,19 +3478,23 @@
       <c r="B19" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="49"/>
+      <c r="C19" s="49">
+        <v>3</v>
+      </c>
       <c r="D19" s="83">
         <f>SUM(G19:BJ19)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E19" s="50"/>
       <c r="F19" s="51"/>
       <c r="G19" s="53"/>
       <c r="H19" s="54"/>
       <c r="I19" s="55"/>
-      <c r="J19" s="55"/>
+      <c r="J19" s="55">
+        <v>2</v>
+      </c>
       <c r="K19" s="56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L19" s="57"/>
       <c r="M19" s="58"/>
@@ -3492,9 +3514,9 @@
       <c r="AA19" s="58"/>
       <c r="AB19" s="53"/>
       <c r="AC19" s="54"/>
-      <c r="AD19" s="55"/>
-      <c r="AE19" s="55"/>
-      <c r="AF19" s="56"/>
+      <c r="AD19" s="54"/>
+      <c r="AE19" s="54"/>
+      <c r="AF19" s="54"/>
       <c r="AG19" s="57"/>
       <c r="AH19" s="58"/>
       <c r="AI19" s="53"/>
@@ -3533,10 +3555,12 @@
       <c r="B20" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="49"/>
+      <c r="C20" s="49">
+        <v>10</v>
+      </c>
       <c r="D20" s="83">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="51"/>
@@ -3544,10 +3568,10 @@
       <c r="H20" s="60"/>
       <c r="I20" s="55"/>
       <c r="J20" s="55">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K20" s="56">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L20" s="57"/>
       <c r="M20" s="58"/>
@@ -3567,9 +3591,9 @@
       <c r="AA20" s="58"/>
       <c r="AB20" s="59"/>
       <c r="AC20" s="60"/>
-      <c r="AD20" s="55"/>
-      <c r="AE20" s="55"/>
-      <c r="AF20" s="56"/>
+      <c r="AD20" s="60"/>
+      <c r="AE20" s="60"/>
+      <c r="AF20" s="60"/>
       <c r="AG20" s="57"/>
       <c r="AH20" s="58"/>
       <c r="AI20" s="59"/>
@@ -3608,7 +3632,9 @@
       <c r="B21" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="49"/>
+      <c r="C21" s="49">
+        <v>8</v>
+      </c>
       <c r="D21" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3625,7 +3651,7 @@
       <c r="N21" s="59"/>
       <c r="O21" s="60"/>
       <c r="P21" s="55"/>
-      <c r="Q21" s="55"/>
+      <c r="Q21" s="63"/>
       <c r="R21" s="56"/>
       <c r="S21" s="57"/>
       <c r="T21" s="58"/>
@@ -3638,9 +3664,9 @@
       <c r="AA21" s="58"/>
       <c r="AB21" s="59"/>
       <c r="AC21" s="60"/>
-      <c r="AD21" s="55"/>
-      <c r="AE21" s="55"/>
-      <c r="AF21" s="56"/>
+      <c r="AD21" s="60"/>
+      <c r="AE21" s="60"/>
+      <c r="AF21" s="60"/>
       <c r="AG21" s="57"/>
       <c r="AH21" s="58"/>
       <c r="AI21" s="59"/>
@@ -3679,7 +3705,9 @@
       <c r="B22" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="49"/>
+      <c r="C22" s="49">
+        <v>6</v>
+      </c>
       <c r="D22" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3697,7 +3725,7 @@
       <c r="O22" s="60"/>
       <c r="P22" s="55"/>
       <c r="Q22" s="55"/>
-      <c r="R22" s="56"/>
+      <c r="R22" s="63"/>
       <c r="S22" s="57"/>
       <c r="T22" s="58"/>
       <c r="U22" s="59"/>
@@ -3707,11 +3735,11 @@
       <c r="Y22" s="56"/>
       <c r="Z22" s="57"/>
       <c r="AA22" s="58"/>
-      <c r="AB22" s="59"/>
-      <c r="AC22" s="60"/>
-      <c r="AD22" s="55"/>
-      <c r="AE22" s="55"/>
-      <c r="AF22" s="56"/>
+      <c r="AB22" s="53"/>
+      <c r="AC22" s="54"/>
+      <c r="AD22" s="54"/>
+      <c r="AE22" s="54"/>
+      <c r="AF22" s="54"/>
       <c r="AG22" s="57"/>
       <c r="AH22" s="58"/>
       <c r="AI22" s="59"/>
@@ -3750,7 +3778,9 @@
       <c r="B23" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="49"/>
+      <c r="C23" s="49">
+        <v>8</v>
+      </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3780,9 +3810,9 @@
       <c r="AA23" s="58"/>
       <c r="AB23" s="59"/>
       <c r="AC23" s="60"/>
-      <c r="AD23" s="61"/>
-      <c r="AE23" s="61"/>
-      <c r="AF23" s="56"/>
+      <c r="AD23" s="60"/>
+      <c r="AE23" s="60"/>
+      <c r="AF23" s="60"/>
       <c r="AG23" s="57"/>
       <c r="AH23" s="58"/>
       <c r="AI23" s="59"/>
@@ -3821,7 +3851,9 @@
       <c r="B24" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="49"/>
+      <c r="C24" s="49">
+        <v>4</v>
+      </c>
       <c r="D24" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3851,9 +3883,9 @@
       <c r="AA24" s="58"/>
       <c r="AB24" s="59"/>
       <c r="AC24" s="60"/>
-      <c r="AD24" s="55"/>
-      <c r="AE24" s="55"/>
-      <c r="AF24" s="56"/>
+      <c r="AD24" s="60"/>
+      <c r="AE24" s="60"/>
+      <c r="AF24" s="60"/>
       <c r="AG24" s="57"/>
       <c r="AH24" s="58"/>
       <c r="AI24" s="59"/>
@@ -3892,7 +3924,9 @@
       <c r="B25" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="49"/>
+      <c r="C25" s="49">
+        <v>5</v>
+      </c>
       <c r="D25" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3920,11 +3954,11 @@
       <c r="Y25" s="56"/>
       <c r="Z25" s="57"/>
       <c r="AA25" s="58"/>
-      <c r="AB25" s="59"/>
-      <c r="AC25" s="60"/>
-      <c r="AD25" s="55"/>
-      <c r="AE25" s="55"/>
-      <c r="AF25" s="56"/>
+      <c r="AB25" s="53"/>
+      <c r="AC25" s="54"/>
+      <c r="AD25" s="54"/>
+      <c r="AE25" s="54"/>
+      <c r="AF25" s="54"/>
       <c r="AG25" s="57"/>
       <c r="AH25" s="58"/>
       <c r="AI25" s="59"/>
@@ -3963,7 +3997,9 @@
       <c r="B26" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="49"/>
+      <c r="C26" s="49">
+        <v>10</v>
+      </c>
       <c r="D26" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3993,9 +4029,9 @@
       <c r="AA26" s="58"/>
       <c r="AB26" s="59"/>
       <c r="AC26" s="60"/>
-      <c r="AD26" s="55"/>
-      <c r="AE26" s="55"/>
-      <c r="AF26" s="56"/>
+      <c r="AD26" s="60"/>
+      <c r="AE26" s="60"/>
+      <c r="AF26" s="60"/>
       <c r="AG26" s="57"/>
       <c r="AH26" s="58"/>
       <c r="AI26" s="59"/>
@@ -4034,7 +4070,9 @@
       <c r="B27" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="49"/>
+      <c r="C27" s="49">
+        <v>7</v>
+      </c>
       <c r="D27" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4064,9 +4102,9 @@
       <c r="AA27" s="58"/>
       <c r="AB27" s="59"/>
       <c r="AC27" s="60"/>
-      <c r="AD27" s="55"/>
-      <c r="AE27" s="55"/>
-      <c r="AF27" s="56"/>
+      <c r="AD27" s="60"/>
+      <c r="AE27" s="60"/>
+      <c r="AF27" s="60"/>
       <c r="AG27" s="57"/>
       <c r="AH27" s="58"/>
       <c r="AI27" s="59"/>
@@ -4105,7 +4143,9 @@
       <c r="B28" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="49"/>
+      <c r="C28" s="49">
+        <v>10</v>
+      </c>
       <c r="D28" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4133,11 +4173,11 @@
       <c r="Y28" s="56"/>
       <c r="Z28" s="57"/>
       <c r="AA28" s="58"/>
-      <c r="AB28" s="59"/>
-      <c r="AC28" s="60"/>
-      <c r="AD28" s="55"/>
-      <c r="AE28" s="55"/>
-      <c r="AF28" s="56"/>
+      <c r="AB28" s="53"/>
+      <c r="AC28" s="54"/>
+      <c r="AD28" s="54"/>
+      <c r="AE28" s="54"/>
+      <c r="AF28" s="54"/>
       <c r="AG28" s="57"/>
       <c r="AH28" s="58"/>
       <c r="AI28" s="59"/>
@@ -4176,7 +4216,9 @@
       <c r="B29" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="49"/>
+      <c r="C29" s="49">
+        <v>12</v>
+      </c>
       <c r="D29" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4204,11 +4246,11 @@
       <c r="Y29" s="56"/>
       <c r="Z29" s="57"/>
       <c r="AA29" s="58"/>
-      <c r="AB29" s="71"/>
-      <c r="AC29" s="72"/>
-      <c r="AD29" s="55"/>
-      <c r="AE29" s="55"/>
-      <c r="AF29" s="56"/>
+      <c r="AB29" s="59"/>
+      <c r="AC29" s="60"/>
+      <c r="AD29" s="60"/>
+      <c r="AE29" s="60"/>
+      <c r="AF29" s="60"/>
       <c r="AG29" s="57"/>
       <c r="AH29" s="58"/>
       <c r="AI29" s="71"/>
@@ -4273,11 +4315,11 @@
       <c r="Y30" s="56"/>
       <c r="Z30" s="57"/>
       <c r="AA30" s="58"/>
-      <c r="AB30" s="69"/>
-      <c r="AC30" s="70"/>
-      <c r="AD30" s="55"/>
-      <c r="AE30" s="55"/>
-      <c r="AF30" s="56"/>
+      <c r="AB30" s="59"/>
+      <c r="AC30" s="60"/>
+      <c r="AD30" s="60"/>
+      <c r="AE30" s="60"/>
+      <c r="AF30" s="60"/>
       <c r="AG30" s="57"/>
       <c r="AH30" s="58"/>
       <c r="AI30" s="69"/>
@@ -4420,9 +4462,9 @@
       <c r="AA32" s="58"/>
       <c r="AB32" s="53"/>
       <c r="AC32" s="54"/>
-      <c r="AD32" s="55"/>
-      <c r="AE32" s="55"/>
-      <c r="AF32" s="56"/>
+      <c r="AD32" s="54"/>
+      <c r="AE32" s="54"/>
+      <c r="AF32" s="54"/>
       <c r="AG32" s="57"/>
       <c r="AH32" s="58"/>
       <c r="AI32" s="53"/>
@@ -4491,9 +4533,9 @@
       <c r="AA33" s="58"/>
       <c r="AB33" s="59"/>
       <c r="AC33" s="60"/>
-      <c r="AD33" s="55"/>
-      <c r="AE33" s="55"/>
-      <c r="AF33" s="56"/>
+      <c r="AD33" s="60"/>
+      <c r="AE33" s="60"/>
+      <c r="AF33" s="60"/>
       <c r="AG33" s="57"/>
       <c r="AH33" s="58"/>
       <c r="AI33" s="59"/>
@@ -4562,9 +4604,9 @@
       <c r="AA34" s="58"/>
       <c r="AB34" s="59"/>
       <c r="AC34" s="60"/>
-      <c r="AD34" s="55"/>
-      <c r="AE34" s="55"/>
-      <c r="AF34" s="56"/>
+      <c r="AD34" s="60"/>
+      <c r="AE34" s="60"/>
+      <c r="AF34" s="60"/>
       <c r="AG34" s="57"/>
       <c r="AH34" s="58"/>
       <c r="AI34" s="59"/>
@@ -4629,11 +4671,11 @@
       <c r="Y35" s="56"/>
       <c r="Z35" s="57"/>
       <c r="AA35" s="58"/>
-      <c r="AB35" s="69"/>
-      <c r="AC35" s="70"/>
-      <c r="AD35" s="55"/>
-      <c r="AE35" s="55"/>
-      <c r="AF35" s="56"/>
+      <c r="AB35" s="53"/>
+      <c r="AC35" s="54"/>
+      <c r="AD35" s="54"/>
+      <c r="AE35" s="54"/>
+      <c r="AF35" s="54"/>
       <c r="AG35" s="57"/>
       <c r="AH35" s="58"/>
       <c r="AI35" s="69"/>
@@ -4776,9 +4818,9 @@
       <c r="AA37" s="58"/>
       <c r="AB37" s="53"/>
       <c r="AC37" s="54"/>
-      <c r="AD37" s="55"/>
-      <c r="AE37" s="55"/>
-      <c r="AF37" s="56"/>
+      <c r="AD37" s="54"/>
+      <c r="AE37" s="54"/>
+      <c r="AF37" s="54"/>
       <c r="AG37" s="57"/>
       <c r="AH37" s="58"/>
       <c r="AI37" s="53"/>
@@ -4843,11 +4885,11 @@
       <c r="Y38" s="56"/>
       <c r="Z38" s="57"/>
       <c r="AA38" s="58"/>
-      <c r="AB38" s="69"/>
-      <c r="AC38" s="70"/>
-      <c r="AD38" s="55"/>
-      <c r="AE38" s="55"/>
-      <c r="AF38" s="56"/>
+      <c r="AB38" s="59"/>
+      <c r="AC38" s="60"/>
+      <c r="AD38" s="60"/>
+      <c r="AE38" s="60"/>
+      <c r="AF38" s="60"/>
       <c r="AG38" s="57"/>
       <c r="AH38" s="58"/>
       <c r="AI38" s="69"/>
@@ -4888,7 +4930,7 @@
       </c>
       <c r="C39" s="41">
         <f>SUM(C40:C42)</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="D39" s="42">
         <f>SUM(D40:D42)</f>
@@ -4960,7 +5002,9 @@
       <c r="B40" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="49"/>
+      <c r="C40" s="49">
+        <v>4</v>
+      </c>
       <c r="D40" s="83">
         <f>SUM(G40:BJ40)</f>
         <v>0</v>
@@ -4990,9 +5034,9 @@
       <c r="AA40" s="58"/>
       <c r="AB40" s="53"/>
       <c r="AC40" s="54"/>
-      <c r="AD40" s="55"/>
-      <c r="AE40" s="55"/>
-      <c r="AF40" s="56"/>
+      <c r="AD40" s="54"/>
+      <c r="AE40" s="54"/>
+      <c r="AF40" s="54"/>
       <c r="AG40" s="57"/>
       <c r="AH40" s="58"/>
       <c r="AI40" s="53"/>
@@ -5031,7 +5075,9 @@
       <c r="B41" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="49"/>
+      <c r="C41" s="49">
+        <v>1.5</v>
+      </c>
       <c r="D41" s="83">
         <f t="shared" ref="D41:D42" si="2">SUM(G41:BJ41)</f>
         <v>0</v>
@@ -5061,9 +5107,9 @@
       <c r="AA41" s="58"/>
       <c r="AB41" s="59"/>
       <c r="AC41" s="60"/>
-      <c r="AD41" s="55"/>
-      <c r="AE41" s="55"/>
-      <c r="AF41" s="56"/>
+      <c r="AD41" s="60"/>
+      <c r="AE41" s="60"/>
+      <c r="AF41" s="60"/>
       <c r="AG41" s="57"/>
       <c r="AH41" s="58"/>
       <c r="AI41" s="59"/>
@@ -5128,11 +5174,11 @@
       <c r="Y42" s="56"/>
       <c r="Z42" s="57"/>
       <c r="AA42" s="58"/>
-      <c r="AB42" s="69"/>
-      <c r="AC42" s="70"/>
-      <c r="AD42" s="55"/>
-      <c r="AE42" s="55"/>
-      <c r="AF42" s="56"/>
+      <c r="AB42" s="53"/>
+      <c r="AC42" s="54"/>
+      <c r="AD42" s="54"/>
+      <c r="AE42" s="54"/>
+      <c r="AF42" s="54"/>
       <c r="AG42" s="57"/>
       <c r="AH42" s="58"/>
       <c r="AI42" s="69"/>
@@ -5171,11 +5217,11 @@
       </c>
       <c r="C43" s="37">
         <f>C39+C36+C31+C18+C14+C9</f>
-        <v>5</v>
+        <v>101.5</v>
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5193,11 +5239,11 @@
       </c>
       <c r="J43" s="39">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>7.5</v>
       </c>
       <c r="K43" s="39">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L43" s="39">
         <f t="shared" si="3"/>
@@ -5217,7 +5263,7 @@
       </c>
       <c r="P43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="Q43" s="39">
         <f t="shared" si="3"/>
@@ -5429,6 +5475,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE14E400-DEE2-4E79-8367-AB849CB2C5F0}">
+  <dimension ref="C3:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4">
+        <f>+(D3+2+D4+D5)/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -5469,11 +5549,11 @@
       <c r="B3" s="96"/>
       <c r="C3" s="80">
         <f>Zeitplanung!C9</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" s="80">
         <f>Zeitplanung!D9</f>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
@@ -5486,11 +5566,11 @@
       <c r="B4" s="96"/>
       <c r="C4" s="80">
         <f>Zeitplanung!C14</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4" s="80">
         <f>Zeitplanung!D14</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" s="82"/>
       <c r="F4" s="81"/>
@@ -5503,11 +5583,11 @@
       <c r="B5" s="96"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>
@@ -5552,7 +5632,7 @@
       <c r="B8" s="96"/>
       <c r="C8" s="80">
         <f>Zeitplanung!C39</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="D8" s="80">
         <f>Zeitplanung!D39</f>

</xml_diff>

<commit_message>
Jetzt ist alles fertig
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung Luminescence LED's.xlsx
+++ b/doc/Zeitplanung Luminescence LED's.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr codeName="DieseArbeitsmappe" showPivotChartFilter="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darvi\Documents\Luminescence-LED\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53385A00-AF3A-47AD-9C8F-21CB6A3BFDE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559AA982-5A1C-46D7-ACA7-EE245F9F1214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -198,9 +198,6 @@
     <t xml:space="preserve"> Abwesend (Ferien/Schule)</t>
   </si>
   <si>
-    <t>Deployment  (Installationsanleitung, Setup, etc)</t>
-  </si>
-  <si>
     <t>Project Abstract</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>Worst Case</t>
+  </si>
+  <si>
+    <t>Deployment  (Installation aufbauen, zu Demozwecken)</t>
   </si>
 </sst>
 </file>
@@ -373,7 +373,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,6 +468,17 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="49">
     <border>
@@ -1112,7 +1123,7 @@
     </xf>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1413,6 +1424,106 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="17" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="17" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="17" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="26" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1429,6 +1540,18 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1618,13 +1741,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2131,8 +2254,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="136" zoomScaleNormal="136" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2142,7 +2265,9 @@
     <col min="3" max="3" width="5.19921875" style="5" customWidth="1"/>
     <col min="4" max="4" width="5.19921875" style="13" customWidth="1"/>
     <col min="5" max="6" width="5.19921875" style="5" customWidth="1"/>
-    <col min="7" max="62" width="2.19921875" style="5" customWidth="1"/>
+    <col min="7" max="27" width="2.19921875" style="5" customWidth="1"/>
+    <col min="28" max="41" width="2.19921875" style="91" customWidth="1"/>
+    <col min="42" max="62" width="2.19921875" style="5" customWidth="1"/>
     <col min="63" max="16384" width="12.5" style="5"/>
   </cols>
   <sheetData>
@@ -2176,9 +2301,9 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
+      <c r="AB1" s="90"/>
+      <c r="AC1" s="90"/>
+      <c r="AD1" s="90"/>
     </row>
     <row r="2" spans="1:62" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
@@ -2208,20 +2333,20 @@
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
       <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="6"/>
-      <c r="AI2" s="6"/>
-      <c r="AJ2" s="6"/>
-      <c r="AK2" s="6"/>
-      <c r="AL2" s="6"/>
-      <c r="AM2" s="6"/>
-      <c r="AN2" s="6"/>
-      <c r="AO2" s="6"/>
+      <c r="AB2" s="92"/>
+      <c r="AC2" s="92"/>
+      <c r="AD2" s="92"/>
+      <c r="AE2" s="92"/>
+      <c r="AF2" s="92"/>
+      <c r="AG2" s="92"/>
+      <c r="AH2" s="92"/>
+      <c r="AI2" s="92"/>
+      <c r="AJ2" s="92"/>
+      <c r="AK2" s="92"/>
+      <c r="AL2" s="92"/>
+      <c r="AM2" s="92"/>
+      <c r="AN2" s="92"/>
+      <c r="AO2" s="92"/>
       <c r="AP2" s="6"/>
       <c r="AQ2" s="6"/>
       <c r="AR2" s="6"/>
@@ -2253,7 +2378,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="86"/>
       <c r="H3" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -2274,20 +2399,20 @@
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
       <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="6"/>
-      <c r="AJ3" s="6"/>
-      <c r="AK3" s="6"/>
-      <c r="AL3" s="6"/>
-      <c r="AM3" s="6"/>
-      <c r="AN3" s="6"/>
-      <c r="AO3" s="6"/>
+      <c r="AB3" s="92"/>
+      <c r="AC3" s="92"/>
+      <c r="AD3" s="92"/>
+      <c r="AE3" s="92"/>
+      <c r="AF3" s="92"/>
+      <c r="AG3" s="92"/>
+      <c r="AH3" s="92"/>
+      <c r="AI3" s="92"/>
+      <c r="AJ3" s="92"/>
+      <c r="AK3" s="92"/>
+      <c r="AL3" s="92"/>
+      <c r="AM3" s="92"/>
+      <c r="AN3" s="92"/>
+      <c r="AO3" s="92"/>
       <c r="AP3" s="6"/>
       <c r="AQ3" s="6"/>
       <c r="AR3" s="6"/>
@@ -2338,20 +2463,20 @@
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
       <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="6"/>
-      <c r="AF4" s="6"/>
-      <c r="AG4" s="6"/>
-      <c r="AH4" s="6"/>
-      <c r="AI4" s="6"/>
-      <c r="AJ4" s="6"/>
-      <c r="AK4" s="6"/>
-      <c r="AL4" s="6"/>
-      <c r="AM4" s="6"/>
-      <c r="AN4" s="6"/>
-      <c r="AO4" s="6"/>
+      <c r="AB4" s="92"/>
+      <c r="AC4" s="92"/>
+      <c r="AD4" s="92"/>
+      <c r="AE4" s="92"/>
+      <c r="AF4" s="92"/>
+      <c r="AG4" s="92"/>
+      <c r="AH4" s="92"/>
+      <c r="AI4" s="92"/>
+      <c r="AJ4" s="92"/>
+      <c r="AK4" s="92"/>
+      <c r="AL4" s="92"/>
+      <c r="AM4" s="92"/>
+      <c r="AN4" s="92"/>
+      <c r="AO4" s="92"/>
       <c r="AP4" s="6"/>
       <c r="AQ4" s="6"/>
       <c r="AR4" s="6"/>
@@ -2404,20 +2529,20 @@
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
-      <c r="AG5" s="6"/>
-      <c r="AH5" s="6"/>
-      <c r="AI5" s="6"/>
-      <c r="AJ5" s="6"/>
-      <c r="AK5" s="6"/>
-      <c r="AL5" s="6"/>
-      <c r="AM5" s="6"/>
-      <c r="AN5" s="6"/>
-      <c r="AO5" s="6"/>
+      <c r="AB5" s="92"/>
+      <c r="AC5" s="92"/>
+      <c r="AD5" s="92"/>
+      <c r="AE5" s="92"/>
+      <c r="AF5" s="92"/>
+      <c r="AG5" s="92"/>
+      <c r="AH5" s="92"/>
+      <c r="AI5" s="92"/>
+      <c r="AJ5" s="92"/>
+      <c r="AK5" s="92"/>
+      <c r="AL5" s="92"/>
+      <c r="AM5" s="92"/>
+      <c r="AN5" s="92"/>
+      <c r="AO5" s="92"/>
       <c r="AP5" s="6"/>
       <c r="AQ5" s="6"/>
       <c r="AR5" s="6"/>
@@ -2451,88 +2576,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="90" t="s">
+      <c r="C7" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="90"/>
+      <c r="D7" s="117"/>
       <c r="E7" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="91" t="s">
+      <c r="G7" s="118" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="118"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="118"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="118"/>
+      <c r="M7" s="119"/>
+      <c r="N7" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="91"/>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
-      <c r="L7" s="91"/>
-      <c r="M7" s="92"/>
-      <c r="N7" s="91" t="s">
+      <c r="O7" s="118"/>
+      <c r="P7" s="118"/>
+      <c r="Q7" s="118"/>
+      <c r="R7" s="118"/>
+      <c r="S7" s="118"/>
+      <c r="T7" s="119"/>
+      <c r="U7" s="118" t="s">
         <v>46</v>
       </c>
-      <c r="O7" s="91"/>
-      <c r="P7" s="91"/>
-      <c r="Q7" s="91"/>
-      <c r="R7" s="91"/>
-      <c r="S7" s="91"/>
-      <c r="T7" s="92"/>
-      <c r="U7" s="91" t="s">
+      <c r="V7" s="118"/>
+      <c r="W7" s="118"/>
+      <c r="X7" s="118"/>
+      <c r="Y7" s="118"/>
+      <c r="Z7" s="118"/>
+      <c r="AA7" s="119"/>
+      <c r="AB7" s="122" t="s">
         <v>47</v>
       </c>
-      <c r="V7" s="91"/>
-      <c r="W7" s="91"/>
-      <c r="X7" s="91"/>
-      <c r="Y7" s="91"/>
-      <c r="Z7" s="91"/>
-      <c r="AA7" s="92"/>
-      <c r="AB7" s="93" t="s">
+      <c r="AC7" s="123"/>
+      <c r="AD7" s="123"/>
+      <c r="AE7" s="123"/>
+      <c r="AF7" s="123"/>
+      <c r="AG7" s="123"/>
+      <c r="AH7" s="124"/>
+      <c r="AI7" s="123" t="s">
         <v>48</v>
       </c>
-      <c r="AC7" s="91"/>
-      <c r="AD7" s="91"/>
-      <c r="AE7" s="91"/>
-      <c r="AF7" s="91"/>
-      <c r="AG7" s="91"/>
-      <c r="AH7" s="92"/>
-      <c r="AI7" s="91" t="s">
+      <c r="AJ7" s="123"/>
+      <c r="AK7" s="123"/>
+      <c r="AL7" s="123"/>
+      <c r="AM7" s="123"/>
+      <c r="AN7" s="123"/>
+      <c r="AO7" s="124"/>
+      <c r="AP7" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="AJ7" s="91"/>
-      <c r="AK7" s="91"/>
-      <c r="AL7" s="91"/>
-      <c r="AM7" s="91"/>
-      <c r="AN7" s="91"/>
-      <c r="AO7" s="92"/>
-      <c r="AP7" s="93" t="s">
+      <c r="AQ7" s="118"/>
+      <c r="AR7" s="118"/>
+      <c r="AS7" s="118"/>
+      <c r="AT7" s="118"/>
+      <c r="AU7" s="118"/>
+      <c r="AV7" s="119"/>
+      <c r="AW7" s="118" t="s">
         <v>50</v>
       </c>
-      <c r="AQ7" s="91"/>
-      <c r="AR7" s="91"/>
-      <c r="AS7" s="91"/>
-      <c r="AT7" s="91"/>
-      <c r="AU7" s="91"/>
-      <c r="AV7" s="92"/>
-      <c r="AW7" s="91" t="s">
+      <c r="AX7" s="118"/>
+      <c r="AY7" s="118"/>
+      <c r="AZ7" s="118"/>
+      <c r="BA7" s="118"/>
+      <c r="BB7" s="118"/>
+      <c r="BC7" s="119"/>
+      <c r="BD7" s="120" t="s">
         <v>51</v>
       </c>
-      <c r="AX7" s="91"/>
-      <c r="AY7" s="91"/>
-      <c r="AZ7" s="91"/>
-      <c r="BA7" s="91"/>
-      <c r="BB7" s="91"/>
-      <c r="BC7" s="92"/>
-      <c r="BD7" s="93" t="s">
-        <v>52</v>
-      </c>
-      <c r="BE7" s="91"/>
-      <c r="BF7" s="91"/>
-      <c r="BG7" s="91"/>
-      <c r="BH7" s="91"/>
-      <c r="BI7" s="91"/>
-      <c r="BJ7" s="94"/>
+      <c r="BE7" s="118"/>
+      <c r="BF7" s="118"/>
+      <c r="BG7" s="118"/>
+      <c r="BH7" s="118"/>
+      <c r="BI7" s="118"/>
+      <c r="BJ7" s="121"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -2549,7 +2674,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>17</v>
@@ -2614,46 +2739,46 @@
       <c r="AA8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="AB8" s="16" t="s">
+      <c r="AB8" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="AC8" s="15" t="s">
+      <c r="AC8" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="AD8" s="15" t="s">
+      <c r="AD8" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="AE8" s="14" t="s">
+      <c r="AE8" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="AF8" s="14" t="s">
+      <c r="AF8" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="AG8" s="17" t="s">
+      <c r="AG8" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="AH8" s="18" t="s">
+      <c r="AH8" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="AI8" s="16" t="s">
+      <c r="AI8" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="AJ8" s="15" t="s">
+      <c r="AJ8" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="AK8" s="15" t="s">
+      <c r="AK8" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="AL8" s="14" t="s">
+      <c r="AL8" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="AM8" s="14" t="s">
+      <c r="AM8" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="AN8" s="17" t="s">
+      <c r="AN8" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="AO8" s="18" t="s">
+      <c r="AO8" s="96" t="s">
         <v>20</v>
       </c>
       <c r="AP8" s="16" t="s">
@@ -2733,7 +2858,7 @@
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -2758,20 +2883,20 @@
       <c r="Y9" s="74"/>
       <c r="Z9" s="75"/>
       <c r="AA9" s="76"/>
-      <c r="AB9" s="77"/>
-      <c r="AC9" s="74"/>
-      <c r="AD9" s="74"/>
-      <c r="AE9" s="74"/>
-      <c r="AF9" s="75"/>
-      <c r="AG9" s="75"/>
-      <c r="AH9" s="76"/>
-      <c r="AI9" s="73"/>
-      <c r="AJ9" s="74"/>
-      <c r="AK9" s="74"/>
-      <c r="AL9" s="74"/>
-      <c r="AM9" s="75"/>
-      <c r="AN9" s="75"/>
-      <c r="AO9" s="76"/>
+      <c r="AB9" s="97"/>
+      <c r="AC9" s="98"/>
+      <c r="AD9" s="98"/>
+      <c r="AE9" s="98"/>
+      <c r="AF9" s="99"/>
+      <c r="AG9" s="99"/>
+      <c r="AH9" s="100"/>
+      <c r="AI9" s="101"/>
+      <c r="AJ9" s="98"/>
+      <c r="AK9" s="98"/>
+      <c r="AL9" s="98"/>
+      <c r="AM9" s="99"/>
+      <c r="AN9" s="99"/>
+      <c r="AO9" s="100"/>
       <c r="AP9" s="73"/>
       <c r="AQ9" s="74"/>
       <c r="AR9" s="74"/>
@@ -2802,14 +2927,14 @@
         <v>12</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="84"/>
       <c r="E10" s="48">
         <v>1</v>
       </c>
       <c r="F10" s="88" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" s="53"/>
       <c r="H10" s="54"/>
@@ -2832,20 +2957,20 @@
       <c r="Y10" s="56"/>
       <c r="Z10" s="57"/>
       <c r="AA10" s="58"/>
-      <c r="AB10" s="53"/>
-      <c r="AC10" s="54"/>
-      <c r="AD10" s="54"/>
-      <c r="AE10" s="54"/>
-      <c r="AF10" s="54"/>
-      <c r="AG10" s="57"/>
-      <c r="AH10" s="58"/>
-      <c r="AI10" s="53"/>
-      <c r="AJ10" s="54"/>
-      <c r="AK10" s="55"/>
-      <c r="AL10" s="55"/>
-      <c r="AM10" s="56"/>
-      <c r="AN10" s="57"/>
-      <c r="AO10" s="58"/>
+      <c r="AB10" s="102"/>
+      <c r="AC10" s="103"/>
+      <c r="AD10" s="103"/>
+      <c r="AE10" s="103"/>
+      <c r="AF10" s="103"/>
+      <c r="AG10" s="104"/>
+      <c r="AH10" s="105"/>
+      <c r="AI10" s="102"/>
+      <c r="AJ10" s="103"/>
+      <c r="AK10" s="106"/>
+      <c r="AL10" s="106"/>
+      <c r="AM10" s="104"/>
+      <c r="AN10" s="104"/>
+      <c r="AO10" s="105"/>
       <c r="AP10" s="53"/>
       <c r="AQ10" s="54"/>
       <c r="AR10" s="55"/>
@@ -2873,14 +2998,14 @@
         <v>102</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="49">
         <v>3</v>
       </c>
       <c r="D11" s="83">
         <f>SUM(G11:BJ11)</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E11" s="50">
         <v>1</v>
@@ -2900,7 +3025,7 @@
       <c r="N11" s="59"/>
       <c r="O11" s="60"/>
       <c r="P11" s="61">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="61"/>
       <c r="R11" s="56"/>
@@ -2915,20 +3040,20 @@
       <c r="Y11" s="56"/>
       <c r="Z11" s="57"/>
       <c r="AA11" s="58"/>
-      <c r="AB11" s="59"/>
-      <c r="AC11" s="60"/>
-      <c r="AD11" s="60"/>
-      <c r="AE11" s="60"/>
-      <c r="AF11" s="60"/>
-      <c r="AG11" s="57"/>
-      <c r="AH11" s="58"/>
-      <c r="AI11" s="59"/>
-      <c r="AJ11" s="60"/>
-      <c r="AK11" s="61"/>
-      <c r="AL11" s="61"/>
-      <c r="AM11" s="56"/>
-      <c r="AN11" s="57"/>
-      <c r="AO11" s="58"/>
+      <c r="AB11" s="107"/>
+      <c r="AC11" s="108"/>
+      <c r="AD11" s="108"/>
+      <c r="AE11" s="108"/>
+      <c r="AF11" s="108"/>
+      <c r="AG11" s="104"/>
+      <c r="AH11" s="105"/>
+      <c r="AI11" s="107"/>
+      <c r="AJ11" s="108"/>
+      <c r="AK11" s="109"/>
+      <c r="AL11" s="109"/>
+      <c r="AM11" s="104"/>
+      <c r="AN11" s="104"/>
+      <c r="AO11" s="105"/>
       <c r="AP11" s="59"/>
       <c r="AQ11" s="60"/>
       <c r="AR11" s="61"/>
@@ -2963,7 +3088,7 @@
       </c>
       <c r="D12" s="83">
         <f>SUM(G12:BJ12)</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E12" s="50">
         <v>1</v>
@@ -2980,7 +3105,9 @@
       <c r="M12" s="58"/>
       <c r="N12" s="59"/>
       <c r="O12" s="60"/>
-      <c r="P12" s="61"/>
+      <c r="P12" s="61">
+        <v>0.75</v>
+      </c>
       <c r="Q12" s="61"/>
       <c r="R12" s="63"/>
       <c r="S12" s="57"/>
@@ -2992,20 +3119,20 @@
       <c r="Y12" s="63"/>
       <c r="Z12" s="57"/>
       <c r="AA12" s="58"/>
-      <c r="AB12" s="59"/>
-      <c r="AC12" s="60"/>
-      <c r="AD12" s="60"/>
-      <c r="AE12" s="60"/>
-      <c r="AF12" s="60"/>
-      <c r="AG12" s="57"/>
-      <c r="AH12" s="58"/>
-      <c r="AI12" s="59"/>
-      <c r="AJ12" s="60"/>
-      <c r="AK12" s="61"/>
-      <c r="AL12" s="61"/>
-      <c r="AM12" s="63"/>
-      <c r="AN12" s="57"/>
-      <c r="AO12" s="58"/>
+      <c r="AB12" s="107"/>
+      <c r="AC12" s="108"/>
+      <c r="AD12" s="108"/>
+      <c r="AE12" s="108"/>
+      <c r="AF12" s="108"/>
+      <c r="AG12" s="104"/>
+      <c r="AH12" s="105"/>
+      <c r="AI12" s="107"/>
+      <c r="AJ12" s="108"/>
+      <c r="AK12" s="109"/>
+      <c r="AL12" s="109"/>
+      <c r="AM12" s="104"/>
+      <c r="AN12" s="104"/>
+      <c r="AO12" s="105"/>
       <c r="AP12" s="59"/>
       <c r="AQ12" s="60"/>
       <c r="AR12" s="61"/>
@@ -3033,17 +3160,17 @@
         <v>104</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="83"/>
       <c r="E13" s="50">
         <v>1</v>
       </c>
       <c r="F13" s="88" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="59"/>
       <c r="H13" s="60"/>
@@ -3066,25 +3193,25 @@
       <c r="Y13" s="55"/>
       <c r="Z13" s="66"/>
       <c r="AA13" s="67"/>
-      <c r="AB13" s="59"/>
-      <c r="AC13" s="60"/>
-      <c r="AD13" s="60"/>
-      <c r="AE13" s="60"/>
-      <c r="AF13" s="60"/>
-      <c r="AG13" s="57"/>
-      <c r="AH13" s="58"/>
-      <c r="AI13" s="59"/>
-      <c r="AJ13" s="60"/>
-      <c r="AK13" s="55"/>
-      <c r="AL13" s="55"/>
-      <c r="AM13" s="55"/>
-      <c r="AN13" s="66"/>
-      <c r="AO13" s="67"/>
+      <c r="AB13" s="107"/>
+      <c r="AC13" s="108"/>
+      <c r="AD13" s="108"/>
+      <c r="AE13" s="108"/>
+      <c r="AF13" s="108"/>
+      <c r="AG13" s="104"/>
+      <c r="AH13" s="105"/>
+      <c r="AI13" s="107"/>
+      <c r="AJ13" s="108"/>
+      <c r="AK13" s="106"/>
+      <c r="AL13" s="106"/>
+      <c r="AM13" s="106"/>
+      <c r="AN13" s="115"/>
+      <c r="AO13" s="116"/>
       <c r="AP13" s="59"/>
       <c r="AQ13" s="60"/>
       <c r="AR13" s="55"/>
-      <c r="AS13" s="87"/>
-      <c r="AT13" s="55"/>
+      <c r="AS13" s="61"/>
+      <c r="AT13" s="87"/>
       <c r="AU13" s="66"/>
       <c r="AV13" s="67"/>
       <c r="AW13" s="59"/>
@@ -3140,20 +3267,20 @@
       <c r="Y14" s="74"/>
       <c r="Z14" s="75"/>
       <c r="AA14" s="76"/>
-      <c r="AB14" s="77"/>
-      <c r="AC14" s="74"/>
-      <c r="AD14" s="74"/>
-      <c r="AE14" s="74"/>
-      <c r="AF14" s="75"/>
-      <c r="AG14" s="75"/>
-      <c r="AH14" s="76"/>
-      <c r="AI14" s="73"/>
-      <c r="AJ14" s="74"/>
-      <c r="AK14" s="74"/>
-      <c r="AL14" s="74"/>
-      <c r="AM14" s="75"/>
-      <c r="AN14" s="75"/>
-      <c r="AO14" s="76"/>
+      <c r="AB14" s="97"/>
+      <c r="AC14" s="98"/>
+      <c r="AD14" s="98"/>
+      <c r="AE14" s="98"/>
+      <c r="AF14" s="99"/>
+      <c r="AG14" s="99"/>
+      <c r="AH14" s="100"/>
+      <c r="AI14" s="101"/>
+      <c r="AJ14" s="98"/>
+      <c r="AK14" s="98"/>
+      <c r="AL14" s="98"/>
+      <c r="AM14" s="99"/>
+      <c r="AN14" s="99"/>
+      <c r="AO14" s="100"/>
       <c r="AP14" s="73"/>
       <c r="AQ14" s="74"/>
       <c r="AR14" s="74"/>
@@ -3192,7 +3319,7 @@
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="89" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G15" s="53"/>
       <c r="H15" s="54"/>
@@ -3221,20 +3348,20 @@
       <c r="Y15" s="56"/>
       <c r="Z15" s="57"/>
       <c r="AA15" s="58"/>
-      <c r="AB15" s="53"/>
-      <c r="AC15" s="54"/>
-      <c r="AD15" s="54"/>
-      <c r="AE15" s="54"/>
-      <c r="AF15" s="54"/>
-      <c r="AG15" s="57"/>
-      <c r="AH15" s="58"/>
-      <c r="AI15" s="53"/>
-      <c r="AJ15" s="54"/>
-      <c r="AK15" s="55"/>
-      <c r="AL15" s="55"/>
-      <c r="AM15" s="56"/>
-      <c r="AN15" s="57"/>
-      <c r="AO15" s="58"/>
+      <c r="AB15" s="102"/>
+      <c r="AC15" s="103"/>
+      <c r="AD15" s="103"/>
+      <c r="AE15" s="103"/>
+      <c r="AF15" s="103"/>
+      <c r="AG15" s="104"/>
+      <c r="AH15" s="105"/>
+      <c r="AI15" s="102"/>
+      <c r="AJ15" s="103"/>
+      <c r="AK15" s="106"/>
+      <c r="AL15" s="106"/>
+      <c r="AM15" s="104"/>
+      <c r="AN15" s="104"/>
+      <c r="AO15" s="105"/>
       <c r="AP15" s="53"/>
       <c r="AQ15" s="54"/>
       <c r="AR15" s="55"/>
@@ -3264,7 +3391,9 @@
       <c r="B16" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="49"/>
+      <c r="C16" s="49">
+        <v>0</v>
+      </c>
       <c r="D16" s="83">
         <f>SUM(G16:BJ16)</f>
         <v>0</v>
@@ -3292,20 +3421,20 @@
       <c r="Y16" s="56"/>
       <c r="Z16" s="57"/>
       <c r="AA16" s="58"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="60"/>
-      <c r="AD16" s="60"/>
-      <c r="AE16" s="60"/>
-      <c r="AF16" s="60"/>
-      <c r="AG16" s="57"/>
-      <c r="AH16" s="58"/>
-      <c r="AI16" s="59"/>
-      <c r="AJ16" s="60"/>
-      <c r="AK16" s="55"/>
-      <c r="AL16" s="55"/>
-      <c r="AM16" s="56"/>
-      <c r="AN16" s="57"/>
-      <c r="AO16" s="58"/>
+      <c r="AB16" s="107"/>
+      <c r="AC16" s="108"/>
+      <c r="AD16" s="108"/>
+      <c r="AE16" s="108"/>
+      <c r="AF16" s="108"/>
+      <c r="AG16" s="104"/>
+      <c r="AH16" s="105"/>
+      <c r="AI16" s="107"/>
+      <c r="AJ16" s="108"/>
+      <c r="AK16" s="106"/>
+      <c r="AL16" s="106"/>
+      <c r="AM16" s="104"/>
+      <c r="AN16" s="104"/>
+      <c r="AO16" s="105"/>
       <c r="AP16" s="59"/>
       <c r="AQ16" s="60"/>
       <c r="AR16" s="55"/>
@@ -3361,20 +3490,20 @@
       <c r="Y17" s="56"/>
       <c r="Z17" s="57"/>
       <c r="AA17" s="58"/>
-      <c r="AB17" s="59"/>
-      <c r="AC17" s="60"/>
-      <c r="AD17" s="60"/>
-      <c r="AE17" s="60"/>
-      <c r="AF17" s="60"/>
-      <c r="AG17" s="57"/>
-      <c r="AH17" s="58"/>
-      <c r="AI17" s="69"/>
-      <c r="AJ17" s="70"/>
-      <c r="AK17" s="55"/>
-      <c r="AL17" s="55"/>
-      <c r="AM17" s="56"/>
-      <c r="AN17" s="57"/>
-      <c r="AO17" s="58"/>
+      <c r="AB17" s="107"/>
+      <c r="AC17" s="108"/>
+      <c r="AD17" s="108"/>
+      <c r="AE17" s="108"/>
+      <c r="AF17" s="108"/>
+      <c r="AG17" s="104"/>
+      <c r="AH17" s="105"/>
+      <c r="AI17" s="110"/>
+      <c r="AJ17" s="111"/>
+      <c r="AK17" s="106"/>
+      <c r="AL17" s="106"/>
+      <c r="AM17" s="104"/>
+      <c r="AN17" s="104"/>
+      <c r="AO17" s="105"/>
       <c r="AP17" s="69"/>
       <c r="AQ17" s="70"/>
       <c r="AR17" s="55"/>
@@ -3410,7 +3539,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3435,20 +3564,20 @@
       <c r="Y18" s="74"/>
       <c r="Z18" s="75"/>
       <c r="AA18" s="76"/>
-      <c r="AB18" s="77"/>
-      <c r="AC18" s="74"/>
-      <c r="AD18" s="74"/>
-      <c r="AE18" s="74"/>
-      <c r="AF18" s="75"/>
-      <c r="AG18" s="75"/>
-      <c r="AH18" s="76"/>
-      <c r="AI18" s="73"/>
-      <c r="AJ18" s="74"/>
-      <c r="AK18" s="74"/>
-      <c r="AL18" s="74"/>
-      <c r="AM18" s="75"/>
-      <c r="AN18" s="75"/>
-      <c r="AO18" s="76"/>
+      <c r="AB18" s="97"/>
+      <c r="AC18" s="98"/>
+      <c r="AD18" s="98"/>
+      <c r="AE18" s="98"/>
+      <c r="AF18" s="99"/>
+      <c r="AG18" s="99"/>
+      <c r="AH18" s="100"/>
+      <c r="AI18" s="101"/>
+      <c r="AJ18" s="98"/>
+      <c r="AK18" s="98"/>
+      <c r="AL18" s="98"/>
+      <c r="AM18" s="99"/>
+      <c r="AN18" s="99"/>
+      <c r="AO18" s="100"/>
       <c r="AP18" s="73"/>
       <c r="AQ18" s="74"/>
       <c r="AR18" s="74"/>
@@ -3476,14 +3605,14 @@
         <v>301</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="49">
         <v>3</v>
       </c>
       <c r="D19" s="83">
         <f>SUM(G19:BJ19)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E19" s="50"/>
       <c r="F19" s="51"/>
@@ -3500,7 +3629,9 @@
       <c r="M19" s="58"/>
       <c r="N19" s="53"/>
       <c r="O19" s="54"/>
-      <c r="P19" s="55"/>
+      <c r="P19" s="63">
+        <v>3</v>
+      </c>
       <c r="Q19" s="55"/>
       <c r="R19" s="56"/>
       <c r="S19" s="57"/>
@@ -3512,20 +3643,20 @@
       <c r="Y19" s="56"/>
       <c r="Z19" s="57"/>
       <c r="AA19" s="58"/>
-      <c r="AB19" s="53"/>
-      <c r="AC19" s="54"/>
-      <c r="AD19" s="54"/>
-      <c r="AE19" s="54"/>
-      <c r="AF19" s="54"/>
-      <c r="AG19" s="57"/>
-      <c r="AH19" s="58"/>
-      <c r="AI19" s="53"/>
-      <c r="AJ19" s="54"/>
-      <c r="AK19" s="55"/>
-      <c r="AL19" s="55"/>
-      <c r="AM19" s="56"/>
-      <c r="AN19" s="57"/>
-      <c r="AO19" s="58"/>
+      <c r="AB19" s="102"/>
+      <c r="AC19" s="103"/>
+      <c r="AD19" s="103"/>
+      <c r="AE19" s="103"/>
+      <c r="AF19" s="103"/>
+      <c r="AG19" s="104"/>
+      <c r="AH19" s="105"/>
+      <c r="AI19" s="102"/>
+      <c r="AJ19" s="103"/>
+      <c r="AK19" s="106"/>
+      <c r="AL19" s="106"/>
+      <c r="AM19" s="104"/>
+      <c r="AN19" s="104"/>
+      <c r="AO19" s="105"/>
       <c r="AP19" s="53"/>
       <c r="AQ19" s="54"/>
       <c r="AR19" s="55"/>
@@ -3553,7 +3684,7 @@
         <v>302</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="49">
         <v>10</v>
@@ -3578,8 +3709,8 @@
       <c r="N20" s="59"/>
       <c r="O20" s="60"/>
       <c r="P20" s="55"/>
-      <c r="Q20" s="55"/>
-      <c r="R20" s="56"/>
+      <c r="Q20" s="63"/>
+      <c r="R20" s="63"/>
       <c r="S20" s="57"/>
       <c r="T20" s="58"/>
       <c r="U20" s="59"/>
@@ -3589,20 +3720,20 @@
       <c r="Y20" s="56"/>
       <c r="Z20" s="57"/>
       <c r="AA20" s="58"/>
-      <c r="AB20" s="59"/>
-      <c r="AC20" s="60"/>
-      <c r="AD20" s="60"/>
-      <c r="AE20" s="60"/>
-      <c r="AF20" s="60"/>
-      <c r="AG20" s="57"/>
-      <c r="AH20" s="58"/>
-      <c r="AI20" s="59"/>
-      <c r="AJ20" s="60"/>
-      <c r="AK20" s="55"/>
-      <c r="AL20" s="55"/>
-      <c r="AM20" s="56"/>
-      <c r="AN20" s="57"/>
-      <c r="AO20" s="58"/>
+      <c r="AB20" s="107"/>
+      <c r="AC20" s="108"/>
+      <c r="AD20" s="108"/>
+      <c r="AE20" s="108"/>
+      <c r="AF20" s="108"/>
+      <c r="AG20" s="104"/>
+      <c r="AH20" s="105"/>
+      <c r="AI20" s="107"/>
+      <c r="AJ20" s="108"/>
+      <c r="AK20" s="106"/>
+      <c r="AL20" s="106"/>
+      <c r="AM20" s="104"/>
+      <c r="AN20" s="104"/>
+      <c r="AO20" s="105"/>
       <c r="AP20" s="59"/>
       <c r="AQ20" s="60"/>
       <c r="AR20" s="55"/>
@@ -3652,7 +3783,7 @@
       <c r="O21" s="60"/>
       <c r="P21" s="55"/>
       <c r="Q21" s="63"/>
-      <c r="R21" s="56"/>
+      <c r="R21" s="63"/>
       <c r="S21" s="57"/>
       <c r="T21" s="58"/>
       <c r="U21" s="59"/>
@@ -3662,20 +3793,20 @@
       <c r="Y21" s="56"/>
       <c r="Z21" s="57"/>
       <c r="AA21" s="58"/>
-      <c r="AB21" s="59"/>
-      <c r="AC21" s="60"/>
-      <c r="AD21" s="60"/>
-      <c r="AE21" s="60"/>
-      <c r="AF21" s="60"/>
-      <c r="AG21" s="57"/>
-      <c r="AH21" s="58"/>
-      <c r="AI21" s="59"/>
-      <c r="AJ21" s="60"/>
-      <c r="AK21" s="55"/>
-      <c r="AL21" s="55"/>
-      <c r="AM21" s="56"/>
-      <c r="AN21" s="57"/>
-      <c r="AO21" s="58"/>
+      <c r="AB21" s="107"/>
+      <c r="AC21" s="108"/>
+      <c r="AD21" s="108"/>
+      <c r="AE21" s="108"/>
+      <c r="AF21" s="108"/>
+      <c r="AG21" s="104"/>
+      <c r="AH21" s="105"/>
+      <c r="AI21" s="107"/>
+      <c r="AJ21" s="108"/>
+      <c r="AK21" s="106"/>
+      <c r="AL21" s="106"/>
+      <c r="AM21" s="104"/>
+      <c r="AN21" s="104"/>
+      <c r="AO21" s="105"/>
       <c r="AP21" s="59"/>
       <c r="AQ21" s="60"/>
       <c r="AR21" s="55"/>
@@ -3730,25 +3861,25 @@
       <c r="T22" s="58"/>
       <c r="U22" s="59"/>
       <c r="V22" s="60"/>
-      <c r="W22" s="55"/>
+      <c r="W22" s="87"/>
       <c r="X22" s="55"/>
       <c r="Y22" s="56"/>
       <c r="Z22" s="57"/>
       <c r="AA22" s="58"/>
-      <c r="AB22" s="53"/>
-      <c r="AC22" s="54"/>
-      <c r="AD22" s="54"/>
-      <c r="AE22" s="54"/>
-      <c r="AF22" s="54"/>
-      <c r="AG22" s="57"/>
-      <c r="AH22" s="58"/>
-      <c r="AI22" s="59"/>
-      <c r="AJ22" s="60"/>
-      <c r="AK22" s="55"/>
-      <c r="AL22" s="55"/>
-      <c r="AM22" s="56"/>
-      <c r="AN22" s="57"/>
-      <c r="AO22" s="58"/>
+      <c r="AB22" s="102"/>
+      <c r="AC22" s="103"/>
+      <c r="AD22" s="103"/>
+      <c r="AE22" s="103"/>
+      <c r="AF22" s="103"/>
+      <c r="AG22" s="104"/>
+      <c r="AH22" s="105"/>
+      <c r="AI22" s="107"/>
+      <c r="AJ22" s="108"/>
+      <c r="AK22" s="106"/>
+      <c r="AL22" s="106"/>
+      <c r="AM22" s="104"/>
+      <c r="AN22" s="104"/>
+      <c r="AO22" s="105"/>
       <c r="AP22" s="59"/>
       <c r="AQ22" s="60"/>
       <c r="AR22" s="55"/>
@@ -3803,25 +3934,25 @@
       <c r="T23" s="58"/>
       <c r="U23" s="59"/>
       <c r="V23" s="60"/>
-      <c r="W23" s="61"/>
-      <c r="X23" s="61"/>
+      <c r="W23" s="63"/>
+      <c r="X23" s="63"/>
       <c r="Y23" s="56"/>
       <c r="Z23" s="57"/>
       <c r="AA23" s="58"/>
-      <c r="AB23" s="59"/>
-      <c r="AC23" s="60"/>
-      <c r="AD23" s="60"/>
-      <c r="AE23" s="60"/>
-      <c r="AF23" s="60"/>
-      <c r="AG23" s="57"/>
-      <c r="AH23" s="58"/>
-      <c r="AI23" s="59"/>
-      <c r="AJ23" s="60"/>
-      <c r="AK23" s="61"/>
-      <c r="AL23" s="61"/>
-      <c r="AM23" s="56"/>
-      <c r="AN23" s="57"/>
-      <c r="AO23" s="58"/>
+      <c r="AB23" s="107"/>
+      <c r="AC23" s="108"/>
+      <c r="AD23" s="108"/>
+      <c r="AE23" s="108"/>
+      <c r="AF23" s="108"/>
+      <c r="AG23" s="104"/>
+      <c r="AH23" s="105"/>
+      <c r="AI23" s="107"/>
+      <c r="AJ23" s="108"/>
+      <c r="AK23" s="109"/>
+      <c r="AL23" s="109"/>
+      <c r="AM23" s="104"/>
+      <c r="AN23" s="104"/>
+      <c r="AO23" s="105"/>
       <c r="AP23" s="59"/>
       <c r="AQ23" s="60"/>
       <c r="AR23" s="61"/>
@@ -3877,24 +4008,24 @@
       <c r="U24" s="59"/>
       <c r="V24" s="60"/>
       <c r="W24" s="55"/>
-      <c r="X24" s="55"/>
+      <c r="X24" s="63"/>
       <c r="Y24" s="56"/>
       <c r="Z24" s="57"/>
       <c r="AA24" s="58"/>
-      <c r="AB24" s="59"/>
-      <c r="AC24" s="60"/>
-      <c r="AD24" s="60"/>
-      <c r="AE24" s="60"/>
-      <c r="AF24" s="60"/>
-      <c r="AG24" s="57"/>
-      <c r="AH24" s="58"/>
-      <c r="AI24" s="59"/>
-      <c r="AJ24" s="60"/>
-      <c r="AK24" s="55"/>
-      <c r="AL24" s="55"/>
-      <c r="AM24" s="56"/>
-      <c r="AN24" s="57"/>
-      <c r="AO24" s="58"/>
+      <c r="AB24" s="107"/>
+      <c r="AC24" s="108"/>
+      <c r="AD24" s="108"/>
+      <c r="AE24" s="108"/>
+      <c r="AF24" s="108"/>
+      <c r="AG24" s="104"/>
+      <c r="AH24" s="105"/>
+      <c r="AI24" s="107"/>
+      <c r="AJ24" s="108"/>
+      <c r="AK24" s="106"/>
+      <c r="AL24" s="106"/>
+      <c r="AM24" s="104"/>
+      <c r="AN24" s="104"/>
+      <c r="AO24" s="105"/>
       <c r="AP24" s="59"/>
       <c r="AQ24" s="60"/>
       <c r="AR24" s="55"/>
@@ -3951,23 +4082,23 @@
       <c r="V25" s="60"/>
       <c r="W25" s="55"/>
       <c r="X25" s="55"/>
-      <c r="Y25" s="56"/>
+      <c r="Y25" s="63"/>
       <c r="Z25" s="57"/>
       <c r="AA25" s="58"/>
-      <c r="AB25" s="53"/>
-      <c r="AC25" s="54"/>
-      <c r="AD25" s="54"/>
-      <c r="AE25" s="54"/>
-      <c r="AF25" s="54"/>
-      <c r="AG25" s="57"/>
-      <c r="AH25" s="58"/>
-      <c r="AI25" s="59"/>
-      <c r="AJ25" s="60"/>
-      <c r="AK25" s="55"/>
-      <c r="AL25" s="55"/>
-      <c r="AM25" s="56"/>
-      <c r="AN25" s="57"/>
-      <c r="AO25" s="58"/>
+      <c r="AB25" s="63"/>
+      <c r="AC25" s="103"/>
+      <c r="AD25" s="103"/>
+      <c r="AE25" s="103"/>
+      <c r="AF25" s="103"/>
+      <c r="AG25" s="104"/>
+      <c r="AH25" s="105"/>
+      <c r="AI25" s="107"/>
+      <c r="AJ25" s="108"/>
+      <c r="AK25" s="106"/>
+      <c r="AL25" s="106"/>
+      <c r="AM25" s="104"/>
+      <c r="AN25" s="104"/>
+      <c r="AO25" s="105"/>
       <c r="AP25" s="59"/>
       <c r="AQ25" s="60"/>
       <c r="AR25" s="55"/>
@@ -4027,24 +4158,24 @@
       <c r="Y26" s="56"/>
       <c r="Z26" s="57"/>
       <c r="AA26" s="58"/>
-      <c r="AB26" s="59"/>
-      <c r="AC26" s="60"/>
-      <c r="AD26" s="60"/>
-      <c r="AE26" s="60"/>
-      <c r="AF26" s="60"/>
-      <c r="AG26" s="57"/>
-      <c r="AH26" s="58"/>
-      <c r="AI26" s="59"/>
-      <c r="AJ26" s="60"/>
-      <c r="AK26" s="55"/>
-      <c r="AL26" s="55"/>
-      <c r="AM26" s="56"/>
-      <c r="AN26" s="57"/>
-      <c r="AO26" s="58"/>
+      <c r="AB26" s="107"/>
+      <c r="AC26" s="108"/>
+      <c r="AD26" s="108"/>
+      <c r="AE26" s="108"/>
+      <c r="AF26" s="108"/>
+      <c r="AG26" s="104"/>
+      <c r="AH26" s="105"/>
+      <c r="AI26" s="107"/>
+      <c r="AJ26" s="108"/>
+      <c r="AK26" s="106"/>
+      <c r="AL26" s="106"/>
+      <c r="AM26" s="104"/>
+      <c r="AN26" s="104"/>
+      <c r="AO26" s="105"/>
       <c r="AP26" s="59"/>
       <c r="AQ26" s="60"/>
-      <c r="AR26" s="55"/>
-      <c r="AS26" s="55"/>
+      <c r="AR26" s="63"/>
+      <c r="AS26" s="63"/>
       <c r="AT26" s="56"/>
       <c r="AU26" s="57"/>
       <c r="AV26" s="58"/>
@@ -4100,20 +4231,20 @@
       <c r="Y27" s="56"/>
       <c r="Z27" s="57"/>
       <c r="AA27" s="58"/>
-      <c r="AB27" s="59"/>
-      <c r="AC27" s="60"/>
-      <c r="AD27" s="60"/>
-      <c r="AE27" s="60"/>
-      <c r="AF27" s="60"/>
-      <c r="AG27" s="57"/>
-      <c r="AH27" s="58"/>
-      <c r="AI27" s="59"/>
-      <c r="AJ27" s="60"/>
-      <c r="AK27" s="55"/>
-      <c r="AL27" s="55"/>
-      <c r="AM27" s="56"/>
-      <c r="AN27" s="57"/>
-      <c r="AO27" s="58"/>
+      <c r="AB27" s="107"/>
+      <c r="AC27" s="108"/>
+      <c r="AD27" s="108"/>
+      <c r="AE27" s="108"/>
+      <c r="AF27" s="108"/>
+      <c r="AG27" s="104"/>
+      <c r="AH27" s="105"/>
+      <c r="AI27" s="107"/>
+      <c r="AJ27" s="108"/>
+      <c r="AK27" s="106"/>
+      <c r="AL27" s="106"/>
+      <c r="AM27" s="104"/>
+      <c r="AN27" s="104"/>
+      <c r="AO27" s="105"/>
       <c r="AP27" s="59"/>
       <c r="AQ27" s="60"/>
       <c r="AR27" s="55"/>
@@ -4173,20 +4304,20 @@
       <c r="Y28" s="56"/>
       <c r="Z28" s="57"/>
       <c r="AA28" s="58"/>
-      <c r="AB28" s="53"/>
-      <c r="AC28" s="54"/>
-      <c r="AD28" s="54"/>
-      <c r="AE28" s="54"/>
-      <c r="AF28" s="54"/>
-      <c r="AG28" s="57"/>
-      <c r="AH28" s="58"/>
-      <c r="AI28" s="59"/>
-      <c r="AJ28" s="60"/>
-      <c r="AK28" s="55"/>
-      <c r="AL28" s="55"/>
-      <c r="AM28" s="56"/>
-      <c r="AN28" s="57"/>
-      <c r="AO28" s="58"/>
+      <c r="AB28" s="102"/>
+      <c r="AC28" s="103"/>
+      <c r="AD28" s="103"/>
+      <c r="AE28" s="103"/>
+      <c r="AF28" s="103"/>
+      <c r="AG28" s="104"/>
+      <c r="AH28" s="105"/>
+      <c r="AI28" s="107"/>
+      <c r="AJ28" s="108"/>
+      <c r="AK28" s="106"/>
+      <c r="AL28" s="106"/>
+      <c r="AM28" s="104"/>
+      <c r="AN28" s="104"/>
+      <c r="AO28" s="105"/>
       <c r="AP28" s="59"/>
       <c r="AQ28" s="60"/>
       <c r="AR28" s="55"/>
@@ -4246,20 +4377,20 @@
       <c r="Y29" s="56"/>
       <c r="Z29" s="57"/>
       <c r="AA29" s="58"/>
-      <c r="AB29" s="59"/>
-      <c r="AC29" s="60"/>
-      <c r="AD29" s="60"/>
-      <c r="AE29" s="60"/>
-      <c r="AF29" s="60"/>
-      <c r="AG29" s="57"/>
-      <c r="AH29" s="58"/>
-      <c r="AI29" s="71"/>
-      <c r="AJ29" s="72"/>
-      <c r="AK29" s="55"/>
-      <c r="AL29" s="55"/>
-      <c r="AM29" s="56"/>
-      <c r="AN29" s="57"/>
-      <c r="AO29" s="58"/>
+      <c r="AB29" s="107"/>
+      <c r="AC29" s="108"/>
+      <c r="AD29" s="108"/>
+      <c r="AE29" s="108"/>
+      <c r="AF29" s="108"/>
+      <c r="AG29" s="104"/>
+      <c r="AH29" s="105"/>
+      <c r="AI29" s="112"/>
+      <c r="AJ29" s="113"/>
+      <c r="AK29" s="106"/>
+      <c r="AL29" s="106"/>
+      <c r="AM29" s="104"/>
+      <c r="AN29" s="104"/>
+      <c r="AO29" s="105"/>
       <c r="AP29" s="71"/>
       <c r="AQ29" s="72"/>
       <c r="AR29" s="55"/>
@@ -4315,20 +4446,20 @@
       <c r="Y30" s="56"/>
       <c r="Z30" s="57"/>
       <c r="AA30" s="58"/>
-      <c r="AB30" s="59"/>
-      <c r="AC30" s="60"/>
-      <c r="AD30" s="60"/>
-      <c r="AE30" s="60"/>
-      <c r="AF30" s="60"/>
-      <c r="AG30" s="57"/>
-      <c r="AH30" s="58"/>
-      <c r="AI30" s="69"/>
-      <c r="AJ30" s="70"/>
-      <c r="AK30" s="55"/>
-      <c r="AL30" s="55"/>
-      <c r="AM30" s="56"/>
-      <c r="AN30" s="57"/>
-      <c r="AO30" s="58"/>
+      <c r="AB30" s="107"/>
+      <c r="AC30" s="108"/>
+      <c r="AD30" s="108"/>
+      <c r="AE30" s="108"/>
+      <c r="AF30" s="108"/>
+      <c r="AG30" s="104"/>
+      <c r="AH30" s="105"/>
+      <c r="AI30" s="110"/>
+      <c r="AJ30" s="111"/>
+      <c r="AK30" s="106"/>
+      <c r="AL30" s="106"/>
+      <c r="AM30" s="104"/>
+      <c r="AN30" s="104"/>
+      <c r="AO30" s="105"/>
       <c r="AP30" s="69"/>
       <c r="AQ30" s="70"/>
       <c r="AR30" s="55"/>
@@ -4389,20 +4520,20 @@
       <c r="Y31" s="74"/>
       <c r="Z31" s="75"/>
       <c r="AA31" s="76"/>
-      <c r="AB31" s="77"/>
-      <c r="AC31" s="74"/>
-      <c r="AD31" s="74"/>
-      <c r="AE31" s="74"/>
-      <c r="AF31" s="75"/>
-      <c r="AG31" s="75"/>
-      <c r="AH31" s="76"/>
-      <c r="AI31" s="73"/>
-      <c r="AJ31" s="74"/>
-      <c r="AK31" s="74"/>
-      <c r="AL31" s="74"/>
-      <c r="AM31" s="75"/>
-      <c r="AN31" s="75"/>
-      <c r="AO31" s="76"/>
+      <c r="AB31" s="97"/>
+      <c r="AC31" s="98"/>
+      <c r="AD31" s="98"/>
+      <c r="AE31" s="98"/>
+      <c r="AF31" s="99"/>
+      <c r="AG31" s="99"/>
+      <c r="AH31" s="100"/>
+      <c r="AI31" s="101"/>
+      <c r="AJ31" s="98"/>
+      <c r="AK31" s="98"/>
+      <c r="AL31" s="98"/>
+      <c r="AM31" s="99"/>
+      <c r="AN31" s="99"/>
+      <c r="AO31" s="100"/>
       <c r="AP31" s="73"/>
       <c r="AQ31" s="74"/>
       <c r="AR31" s="74"/>
@@ -4460,20 +4591,20 @@
       <c r="Y32" s="56"/>
       <c r="Z32" s="57"/>
       <c r="AA32" s="58"/>
-      <c r="AB32" s="53"/>
-      <c r="AC32" s="54"/>
-      <c r="AD32" s="54"/>
-      <c r="AE32" s="54"/>
-      <c r="AF32" s="54"/>
-      <c r="AG32" s="57"/>
-      <c r="AH32" s="58"/>
-      <c r="AI32" s="53"/>
-      <c r="AJ32" s="54"/>
-      <c r="AK32" s="55"/>
-      <c r="AL32" s="55"/>
-      <c r="AM32" s="56"/>
-      <c r="AN32" s="57"/>
-      <c r="AO32" s="58"/>
+      <c r="AB32" s="102"/>
+      <c r="AC32" s="103"/>
+      <c r="AD32" s="103"/>
+      <c r="AE32" s="103"/>
+      <c r="AF32" s="103"/>
+      <c r="AG32" s="104"/>
+      <c r="AH32" s="105"/>
+      <c r="AI32" s="102"/>
+      <c r="AJ32" s="103"/>
+      <c r="AK32" s="106"/>
+      <c r="AL32" s="106"/>
+      <c r="AM32" s="104"/>
+      <c r="AN32" s="104"/>
+      <c r="AO32" s="105"/>
       <c r="AP32" s="53"/>
       <c r="AQ32" s="54"/>
       <c r="AR32" s="55"/>
@@ -4531,20 +4662,20 @@
       <c r="Y33" s="56"/>
       <c r="Z33" s="57"/>
       <c r="AA33" s="58"/>
-      <c r="AB33" s="59"/>
-      <c r="AC33" s="60"/>
-      <c r="AD33" s="60"/>
-      <c r="AE33" s="60"/>
-      <c r="AF33" s="60"/>
-      <c r="AG33" s="57"/>
-      <c r="AH33" s="58"/>
-      <c r="AI33" s="59"/>
-      <c r="AJ33" s="60"/>
-      <c r="AK33" s="55"/>
-      <c r="AL33" s="55"/>
-      <c r="AM33" s="56"/>
-      <c r="AN33" s="57"/>
-      <c r="AO33" s="58"/>
+      <c r="AB33" s="107"/>
+      <c r="AC33" s="108"/>
+      <c r="AD33" s="108"/>
+      <c r="AE33" s="108"/>
+      <c r="AF33" s="108"/>
+      <c r="AG33" s="104"/>
+      <c r="AH33" s="105"/>
+      <c r="AI33" s="107"/>
+      <c r="AJ33" s="108"/>
+      <c r="AK33" s="106"/>
+      <c r="AL33" s="106"/>
+      <c r="AM33" s="104"/>
+      <c r="AN33" s="104"/>
+      <c r="AO33" s="105"/>
       <c r="AP33" s="59"/>
       <c r="AQ33" s="60"/>
       <c r="AR33" s="55"/>
@@ -4602,20 +4733,20 @@
       <c r="Y34" s="56"/>
       <c r="Z34" s="57"/>
       <c r="AA34" s="58"/>
-      <c r="AB34" s="59"/>
-      <c r="AC34" s="60"/>
-      <c r="AD34" s="60"/>
-      <c r="AE34" s="60"/>
-      <c r="AF34" s="60"/>
-      <c r="AG34" s="57"/>
-      <c r="AH34" s="58"/>
-      <c r="AI34" s="59"/>
-      <c r="AJ34" s="60"/>
-      <c r="AK34" s="55"/>
-      <c r="AL34" s="55"/>
-      <c r="AM34" s="56"/>
-      <c r="AN34" s="57"/>
-      <c r="AO34" s="58"/>
+      <c r="AB34" s="107"/>
+      <c r="AC34" s="108"/>
+      <c r="AD34" s="108"/>
+      <c r="AE34" s="108"/>
+      <c r="AF34" s="108"/>
+      <c r="AG34" s="104"/>
+      <c r="AH34" s="105"/>
+      <c r="AI34" s="107"/>
+      <c r="AJ34" s="108"/>
+      <c r="AK34" s="106"/>
+      <c r="AL34" s="106"/>
+      <c r="AM34" s="104"/>
+      <c r="AN34" s="104"/>
+      <c r="AO34" s="105"/>
       <c r="AP34" s="59"/>
       <c r="AQ34" s="60"/>
       <c r="AR34" s="55"/>
@@ -4671,20 +4802,20 @@
       <c r="Y35" s="56"/>
       <c r="Z35" s="57"/>
       <c r="AA35" s="58"/>
-      <c r="AB35" s="53"/>
-      <c r="AC35" s="54"/>
-      <c r="AD35" s="54"/>
-      <c r="AE35" s="54"/>
-      <c r="AF35" s="54"/>
-      <c r="AG35" s="57"/>
-      <c r="AH35" s="58"/>
-      <c r="AI35" s="69"/>
-      <c r="AJ35" s="70"/>
-      <c r="AK35" s="55"/>
-      <c r="AL35" s="55"/>
-      <c r="AM35" s="56"/>
-      <c r="AN35" s="57"/>
-      <c r="AO35" s="58"/>
+      <c r="AB35" s="102"/>
+      <c r="AC35" s="103"/>
+      <c r="AD35" s="103"/>
+      <c r="AE35" s="103"/>
+      <c r="AF35" s="103"/>
+      <c r="AG35" s="104"/>
+      <c r="AH35" s="105"/>
+      <c r="AI35" s="110"/>
+      <c r="AJ35" s="111"/>
+      <c r="AK35" s="106"/>
+      <c r="AL35" s="106"/>
+      <c r="AM35" s="104"/>
+      <c r="AN35" s="104"/>
+      <c r="AO35" s="105"/>
       <c r="AP35" s="69"/>
       <c r="AQ35" s="70"/>
       <c r="AR35" s="55"/>
@@ -4745,20 +4876,20 @@
       <c r="Y36" s="74"/>
       <c r="Z36" s="75"/>
       <c r="AA36" s="76"/>
-      <c r="AB36" s="77"/>
-      <c r="AC36" s="74"/>
-      <c r="AD36" s="74"/>
-      <c r="AE36" s="74"/>
-      <c r="AF36" s="75"/>
-      <c r="AG36" s="75"/>
-      <c r="AH36" s="76"/>
-      <c r="AI36" s="73"/>
-      <c r="AJ36" s="74"/>
-      <c r="AK36" s="74"/>
-      <c r="AL36" s="74"/>
-      <c r="AM36" s="75"/>
-      <c r="AN36" s="75"/>
-      <c r="AO36" s="76"/>
+      <c r="AB36" s="97"/>
+      <c r="AC36" s="98"/>
+      <c r="AD36" s="98"/>
+      <c r="AE36" s="98"/>
+      <c r="AF36" s="99"/>
+      <c r="AG36" s="99"/>
+      <c r="AH36" s="100"/>
+      <c r="AI36" s="101"/>
+      <c r="AJ36" s="98"/>
+      <c r="AK36" s="98"/>
+      <c r="AL36" s="98"/>
+      <c r="AM36" s="99"/>
+      <c r="AN36" s="99"/>
+      <c r="AO36" s="100"/>
       <c r="AP36" s="73"/>
       <c r="AQ36" s="74"/>
       <c r="AR36" s="74"/>
@@ -4816,20 +4947,20 @@
       <c r="Y37" s="56"/>
       <c r="Z37" s="57"/>
       <c r="AA37" s="58"/>
-      <c r="AB37" s="53"/>
-      <c r="AC37" s="54"/>
-      <c r="AD37" s="54"/>
-      <c r="AE37" s="54"/>
-      <c r="AF37" s="54"/>
-      <c r="AG37" s="57"/>
-      <c r="AH37" s="58"/>
-      <c r="AI37" s="53"/>
-      <c r="AJ37" s="54"/>
-      <c r="AK37" s="55"/>
-      <c r="AL37" s="55"/>
-      <c r="AM37" s="56"/>
-      <c r="AN37" s="57"/>
-      <c r="AO37" s="58"/>
+      <c r="AB37" s="102"/>
+      <c r="AC37" s="103"/>
+      <c r="AD37" s="103"/>
+      <c r="AE37" s="103"/>
+      <c r="AF37" s="103"/>
+      <c r="AG37" s="104"/>
+      <c r="AH37" s="105"/>
+      <c r="AI37" s="102"/>
+      <c r="AJ37" s="103"/>
+      <c r="AK37" s="106"/>
+      <c r="AL37" s="106"/>
+      <c r="AM37" s="104"/>
+      <c r="AN37" s="104"/>
+      <c r="AO37" s="105"/>
       <c r="AP37" s="53"/>
       <c r="AQ37" s="54"/>
       <c r="AR37" s="55"/>
@@ -4885,20 +5016,20 @@
       <c r="Y38" s="56"/>
       <c r="Z38" s="57"/>
       <c r="AA38" s="58"/>
-      <c r="AB38" s="59"/>
-      <c r="AC38" s="60"/>
-      <c r="AD38" s="60"/>
-      <c r="AE38" s="60"/>
-      <c r="AF38" s="60"/>
-      <c r="AG38" s="57"/>
-      <c r="AH38" s="58"/>
-      <c r="AI38" s="69"/>
-      <c r="AJ38" s="70"/>
-      <c r="AK38" s="55"/>
-      <c r="AL38" s="55"/>
-      <c r="AM38" s="56"/>
-      <c r="AN38" s="57"/>
-      <c r="AO38" s="58"/>
+      <c r="AB38" s="107"/>
+      <c r="AC38" s="108"/>
+      <c r="AD38" s="108"/>
+      <c r="AE38" s="108"/>
+      <c r="AF38" s="108"/>
+      <c r="AG38" s="104"/>
+      <c r="AH38" s="105"/>
+      <c r="AI38" s="110"/>
+      <c r="AJ38" s="111"/>
+      <c r="AK38" s="106"/>
+      <c r="AL38" s="106"/>
+      <c r="AM38" s="104"/>
+      <c r="AN38" s="104"/>
+      <c r="AO38" s="105"/>
       <c r="AP38" s="69"/>
       <c r="AQ38" s="70"/>
       <c r="AR38" s="55"/>
@@ -4959,20 +5090,20 @@
       <c r="Y39" s="74"/>
       <c r="Z39" s="75"/>
       <c r="AA39" s="76"/>
-      <c r="AB39" s="77"/>
-      <c r="AC39" s="74"/>
-      <c r="AD39" s="74"/>
-      <c r="AE39" s="74"/>
-      <c r="AF39" s="75"/>
-      <c r="AG39" s="75"/>
-      <c r="AH39" s="76"/>
-      <c r="AI39" s="73"/>
-      <c r="AJ39" s="74"/>
-      <c r="AK39" s="74"/>
-      <c r="AL39" s="74"/>
-      <c r="AM39" s="75"/>
-      <c r="AN39" s="75"/>
-      <c r="AO39" s="76"/>
+      <c r="AB39" s="97"/>
+      <c r="AC39" s="98"/>
+      <c r="AD39" s="98"/>
+      <c r="AE39" s="98"/>
+      <c r="AF39" s="99"/>
+      <c r="AG39" s="99"/>
+      <c r="AH39" s="100"/>
+      <c r="AI39" s="101"/>
+      <c r="AJ39" s="98"/>
+      <c r="AK39" s="98"/>
+      <c r="AL39" s="98"/>
+      <c r="AM39" s="99"/>
+      <c r="AN39" s="99"/>
+      <c r="AO39" s="100"/>
       <c r="AP39" s="73"/>
       <c r="AQ39" s="74"/>
       <c r="AR39" s="74"/>
@@ -5000,7 +5131,7 @@
         <v>601</v>
       </c>
       <c r="B40" s="46" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C40" s="49">
         <v>4</v>
@@ -5032,25 +5163,25 @@
       <c r="Y40" s="56"/>
       <c r="Z40" s="57"/>
       <c r="AA40" s="58"/>
-      <c r="AB40" s="53"/>
-      <c r="AC40" s="54"/>
-      <c r="AD40" s="54"/>
-      <c r="AE40" s="54"/>
-      <c r="AF40" s="54"/>
-      <c r="AG40" s="57"/>
-      <c r="AH40" s="58"/>
-      <c r="AI40" s="53"/>
-      <c r="AJ40" s="54"/>
-      <c r="AK40" s="55"/>
-      <c r="AL40" s="55"/>
-      <c r="AM40" s="56"/>
-      <c r="AN40" s="57"/>
-      <c r="AO40" s="58"/>
+      <c r="AB40" s="102"/>
+      <c r="AC40" s="103"/>
+      <c r="AD40" s="103"/>
+      <c r="AE40" s="103"/>
+      <c r="AF40" s="103"/>
+      <c r="AG40" s="104"/>
+      <c r="AH40" s="105"/>
+      <c r="AI40" s="102"/>
+      <c r="AJ40" s="103"/>
+      <c r="AK40" s="106"/>
+      <c r="AL40" s="106"/>
+      <c r="AM40" s="104"/>
+      <c r="AN40" s="104"/>
+      <c r="AO40" s="105"/>
       <c r="AP40" s="53"/>
       <c r="AQ40" s="54"/>
       <c r="AR40" s="55"/>
       <c r="AS40" s="55"/>
-      <c r="AT40" s="56"/>
+      <c r="AT40" s="63"/>
       <c r="AU40" s="57"/>
       <c r="AV40" s="58"/>
       <c r="AW40" s="53"/>
@@ -5073,7 +5204,7 @@
         <v>602</v>
       </c>
       <c r="B41" s="46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41" s="49">
         <v>1.5</v>
@@ -5105,25 +5236,25 @@
       <c r="Y41" s="56"/>
       <c r="Z41" s="57"/>
       <c r="AA41" s="58"/>
-      <c r="AB41" s="59"/>
-      <c r="AC41" s="60"/>
-      <c r="AD41" s="60"/>
-      <c r="AE41" s="60"/>
-      <c r="AF41" s="60"/>
-      <c r="AG41" s="57"/>
-      <c r="AH41" s="58"/>
-      <c r="AI41" s="59"/>
-      <c r="AJ41" s="60"/>
-      <c r="AK41" s="55"/>
-      <c r="AL41" s="55"/>
-      <c r="AM41" s="56"/>
-      <c r="AN41" s="57"/>
-      <c r="AO41" s="58"/>
+      <c r="AB41" s="107"/>
+      <c r="AC41" s="108"/>
+      <c r="AD41" s="108"/>
+      <c r="AE41" s="108"/>
+      <c r="AF41" s="108"/>
+      <c r="AG41" s="104"/>
+      <c r="AH41" s="105"/>
+      <c r="AI41" s="107"/>
+      <c r="AJ41" s="108"/>
+      <c r="AK41" s="106"/>
+      <c r="AL41" s="106"/>
+      <c r="AM41" s="104"/>
+      <c r="AN41" s="104"/>
+      <c r="AO41" s="105"/>
       <c r="AP41" s="59"/>
       <c r="AQ41" s="60"/>
       <c r="AR41" s="55"/>
       <c r="AS41" s="55"/>
-      <c r="AT41" s="56"/>
+      <c r="AT41" s="63"/>
       <c r="AU41" s="57"/>
       <c r="AV41" s="58"/>
       <c r="AW41" s="59"/>
@@ -5174,20 +5305,20 @@
       <c r="Y42" s="56"/>
       <c r="Z42" s="57"/>
       <c r="AA42" s="58"/>
-      <c r="AB42" s="53"/>
-      <c r="AC42" s="54"/>
-      <c r="AD42" s="54"/>
-      <c r="AE42" s="54"/>
-      <c r="AF42" s="54"/>
-      <c r="AG42" s="57"/>
-      <c r="AH42" s="58"/>
-      <c r="AI42" s="69"/>
-      <c r="AJ42" s="70"/>
-      <c r="AK42" s="55"/>
-      <c r="AL42" s="55"/>
-      <c r="AM42" s="56"/>
-      <c r="AN42" s="57"/>
-      <c r="AO42" s="58"/>
+      <c r="AB42" s="102"/>
+      <c r="AC42" s="103"/>
+      <c r="AD42" s="103"/>
+      <c r="AE42" s="103"/>
+      <c r="AF42" s="103"/>
+      <c r="AG42" s="104"/>
+      <c r="AH42" s="105"/>
+      <c r="AI42" s="110"/>
+      <c r="AJ42" s="111"/>
+      <c r="AK42" s="106"/>
+      <c r="AL42" s="106"/>
+      <c r="AM42" s="104"/>
+      <c r="AN42" s="104"/>
+      <c r="AO42" s="105"/>
       <c r="AP42" s="69"/>
       <c r="AQ42" s="70"/>
       <c r="AR42" s="55"/>
@@ -5221,7 +5352,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>19</v>
+        <v>23.25</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5263,7 +5394,7 @@
       </c>
       <c r="P43" s="39">
         <f t="shared" si="3"/>
-        <v>3.5</v>
+        <v>7.75</v>
       </c>
       <c r="Q43" s="39">
         <f t="shared" si="3"/>
@@ -5309,59 +5440,59 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AB43" s="39">
+      <c r="AB43" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AC43" s="39">
+      <c r="AC43" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AD43" s="39">
+      <c r="AD43" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AE43" s="39">
+      <c r="AE43" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AF43" s="39">
+      <c r="AF43" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AG43" s="39">
+      <c r="AG43" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AH43" s="39">
+      <c r="AH43" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI43" s="39">
+      <c r="AI43" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AJ43" s="39">
+      <c r="AJ43" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AK43" s="39">
+      <c r="AK43" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AL43" s="39">
+      <c r="AL43" s="114">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AM43" s="39">
+      <c r="AM43" s="114">
         <f t="shared" ref="AM43:BD43" si="4">SUM(AM9:AM42)</f>
         <v>0</v>
       </c>
-      <c r="AN43" s="39">
+      <c r="AN43" s="114">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AO43" s="39">
+      <c r="AO43" s="114">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -5486,12 +5617,12 @@
   <sheetData>
     <row r="3" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4">
         <f>+(D3+2+D4+D5)/3</f>
@@ -5500,7 +5631,7 @@
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -5530,10 +5661,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="98"/>
+      <c r="B2" s="128"/>
       <c r="C2" s="79" t="s">
         <v>14</v>
       </c>
@@ -5542,28 +5673,28 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="95" t="str">
+      <c r="A3" s="125" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="96"/>
+      <c r="B3" s="126"/>
       <c r="C3" s="80">
         <f>Zeitplanung!C9</f>
         <v>8</v>
       </c>
       <c r="D3" s="80">
         <f>Zeitplanung!D9</f>
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
     </row>
     <row r="4" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="95" t="str">
+      <c r="A4" s="125" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="96"/>
+      <c r="B4" s="126"/>
       <c r="C4" s="80">
         <f>Zeitplanung!C14</f>
         <v>5</v>
@@ -5576,28 +5707,28 @@
       <c r="F4" s="81"/>
     </row>
     <row r="5" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="95" t="str">
+      <c r="A5" s="125" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="96"/>
+      <c r="B5" s="126"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
         <v>83</v>
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>
     </row>
     <row r="6" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="95" t="str">
+      <c r="A6" s="125" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="96"/>
+      <c r="B6" s="126"/>
       <c r="C6" s="80">
         <f>Zeitplanung!C31</f>
         <v>0</v>
@@ -5609,11 +5740,11 @@
       <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="95" t="str">
+      <c r="A7" s="125" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="96"/>
+      <c r="B7" s="126"/>
       <c r="C7" s="80">
         <f>Zeitplanung!C36</f>
         <v>0</v>
@@ -5625,11 +5756,11 @@
       <c r="F7" s="81"/>
     </row>
     <row r="8" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="95" t="str">
+      <c r="A8" s="125" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="96"/>
+      <c r="B8" s="126"/>
       <c r="C8" s="80">
         <f>Zeitplanung!C39</f>
         <v>5.5</v>

</xml_diff>

<commit_message>
Code vom Sonnenuntergang weitergeführte Dokumente
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung Luminescence LED's.xlsx
+++ b/doc/Zeitplanung Luminescence LED's.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darvi\Documents\Luminescence-LED\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB4A4F6-96AB-493D-9A4C-9F19B6FCB9D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5A5B38-DCBC-473C-B904-49D056E7B315}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1747,7 +1747,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2254,8 +2254,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AJ49" sqref="AJ49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3539,7 +3539,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3612,7 +3612,7 @@
       </c>
       <c r="D19" s="83">
         <f>SUM(G19:BJ19)</f>
-        <v>17</v>
+        <v>53.5</v>
       </c>
       <c r="E19" s="50"/>
       <c r="F19" s="51"/>
@@ -3642,9 +3642,15 @@
       <c r="T19" s="58"/>
       <c r="U19" s="53"/>
       <c r="V19" s="54"/>
-      <c r="W19" s="55"/>
-      <c r="X19" s="55"/>
-      <c r="Y19" s="56"/>
+      <c r="W19" s="55">
+        <v>6</v>
+      </c>
+      <c r="X19" s="55">
+        <v>7</v>
+      </c>
+      <c r="Y19" s="56">
+        <v>7</v>
+      </c>
       <c r="Z19" s="57"/>
       <c r="AA19" s="58"/>
       <c r="AB19" s="102"/>
@@ -3653,7 +3659,9 @@
       <c r="AE19" s="103"/>
       <c r="AF19" s="103"/>
       <c r="AG19" s="104"/>
-      <c r="AH19" s="105"/>
+      <c r="AH19" s="105">
+        <v>4</v>
+      </c>
       <c r="AI19" s="102"/>
       <c r="AJ19" s="103"/>
       <c r="AK19" s="106"/>
@@ -3663,10 +3671,16 @@
       <c r="AO19" s="105"/>
       <c r="AP19" s="53"/>
       <c r="AQ19" s="54"/>
-      <c r="AR19" s="55"/>
-      <c r="AS19" s="55"/>
+      <c r="AR19" s="55">
+        <v>7</v>
+      </c>
+      <c r="AS19" s="55">
+        <v>5</v>
+      </c>
       <c r="AT19" s="56"/>
-      <c r="AU19" s="57"/>
+      <c r="AU19" s="57">
+        <v>0.5</v>
+      </c>
       <c r="AV19" s="58"/>
       <c r="AW19" s="53"/>
       <c r="AX19" s="54"/>
@@ -3695,7 +3709,7 @@
       </c>
       <c r="D20" s="83">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="51"/>
@@ -3723,9 +3737,15 @@
       <c r="T20" s="58"/>
       <c r="U20" s="59"/>
       <c r="V20" s="60"/>
-      <c r="W20" s="55"/>
-      <c r="X20" s="55"/>
-      <c r="Y20" s="56"/>
+      <c r="W20" s="55">
+        <v>2</v>
+      </c>
+      <c r="X20" s="55">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="56">
+        <v>1</v>
+      </c>
       <c r="Z20" s="57"/>
       <c r="AA20" s="58"/>
       <c r="AB20" s="107"/>
@@ -3744,9 +3764,13 @@
       <c r="AO20" s="105"/>
       <c r="AP20" s="59"/>
       <c r="AQ20" s="60"/>
-      <c r="AR20" s="55"/>
+      <c r="AR20" s="55">
+        <v>1</v>
+      </c>
       <c r="AS20" s="55"/>
-      <c r="AT20" s="56"/>
+      <c r="AT20" s="56">
+        <v>3</v>
+      </c>
       <c r="AU20" s="57"/>
       <c r="AV20" s="58"/>
       <c r="AW20" s="59"/>
@@ -3776,7 +3800,7 @@
       </c>
       <c r="D21" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="E21" s="50"/>
       <c r="F21" s="52"/>
@@ -3818,9 +3842,15 @@
       <c r="AP21" s="59"/>
       <c r="AQ21" s="60"/>
       <c r="AR21" s="55"/>
-      <c r="AS21" s="55"/>
-      <c r="AT21" s="56"/>
-      <c r="AU21" s="57"/>
+      <c r="AS21" s="55">
+        <v>3</v>
+      </c>
+      <c r="AT21" s="56">
+        <v>5</v>
+      </c>
+      <c r="AU21" s="57">
+        <v>0.5</v>
+      </c>
       <c r="AV21" s="58"/>
       <c r="AW21" s="59"/>
       <c r="AX21" s="60"/>
@@ -5360,7 +5390,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>39.25</v>
+        <v>92.25</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5430,15 +5460,15 @@
       </c>
       <c r="W43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z43" s="39">
         <f t="shared" si="3"/>
@@ -5474,7 +5504,7 @@
       </c>
       <c r="AH43" s="114">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AI43" s="114">
         <f t="shared" si="3"/>
@@ -5514,19 +5544,19 @@
       </c>
       <c r="AR43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AS43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AT43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AU43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV43" s="39">
         <f t="shared" si="4"/>
@@ -5726,7 +5756,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>